<commit_message>
Updated analysis notebook so that it creates (and uses) pre-processed task metrics.
</commit_message>
<xml_diff>
--- a/Analysis/PostExperiment.xlsx
+++ b/Analysis/PostExperiment.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/euan/Development/Touchless_Slider_Experiment/Analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84BC00F7-8AF3-A34E-9E1E-1FEF6A8EE143}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5DD701B-6668-A44A-82DB-8F9B990154F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22400" yWindow="500" windowWidth="28800" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="52">
   <si>
     <t>ID</t>
   </si>
@@ -145,6 +145,42 @@
   </si>
   <si>
     <t>You had to point and wait and it would sometimes disengage while moving the cursor.</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>Pinch Anywhere;Dwell;Pinch on Circle;Touch In The Air;</t>
+  </si>
+  <si>
+    <t>This interaction was hard to use and the least natural and intuitive method. Its awkward and confusing to use the touch interaction in front of a screen but not touch it, whereas the other techniques feel more connected to the space above the sensor than the display screen. Getting the touch interaction to engage was difficult, but maintaining the touch once engaged was simple and disengaging felt easy.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dwell and pinch anywhere were my favourites, they were intuitive enough that I could focus more on the task and less on performing the gesture, I found dwell easier to use as pinch was hard to get to engage but pinch was better for movement and disengagement </t>
+  </si>
+  <si>
+    <t>Dwell;Pinch Anywhere;Pinch on Circle;Touch In The Air;</t>
+  </si>
+  <si>
+    <t>Dwell was most easy to use because it gave a visual indicator that I was engaged with the slider, and once you understand the limit on speed of movement for your dwell to remain engaged it was very easy to use accurately. Disengaging was somewhat difficult however.</t>
+  </si>
+  <si>
+    <t>touch was difficult to use because the sensor did not always register the touch motion, requiring multiple attempts to engage with the slider circle. This meant if it got lost halfway through the task, reengaging with the bar was frustrating</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Was difficult to control, sensor often wasn't responsive to pinch motion which made it difficult to engage and disengage </t>
+  </si>
+  <si>
+    <t>Easiest to use, benefit of not having to wait to control (like dwell)</t>
+  </si>
+  <si>
+    <t>Most responsive, most intuitive, instantly able to control so easy to correct small errors</t>
+  </si>
+  <si>
+    <t>Often unresponsive to pinch</t>
   </si>
 </sst>
 </file>
@@ -237,8 +273,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:J6" totalsRowShown="0">
-  <autoFilter ref="A1:J6" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:J8" totalsRowShown="0">
+  <autoFilter ref="A1:J8" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID" dataDxfId="9"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Start time" dataDxfId="8"/>
@@ -552,10 +588,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:E1048576"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -755,6 +791,70 @@
         <v>39</v>
       </c>
     </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1">
+        <v>44573.701666666697</v>
+      </c>
+      <c r="C7" s="1">
+        <v>44573.706921296303</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1">
+        <v>44573.742581018501</v>
+      </c>
+      <c r="C8" s="1">
+        <v>44573.746030092603</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
updated post experiment append to concat
</commit_message>
<xml_diff>
--- a/Analysis/PostExperiment.xlsx
+++ b/Analysis/PostExperiment.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="111">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="121">
   <x:si>
     <x:t xml:space="preserve">ID</x:t>
   </x:si>
@@ -358,6 +358,36 @@
   </x:si>
   <x:si>
     <x:t xml:space="preserve">It kept stopping and starting and was difficult to control</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">18</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">it was time consuming</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">It was easier</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">because it was the easiest</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Because it was the hardest and most time consuming</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">19</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">I lost control quickly, activation takes time</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Quick, the fact your hand can be anywhere</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">no specific hand position needed</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">I needed to get really close to the screen</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -454,8 +484,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:L18" insertRow="1" totalsRowShown="0">
-  <x:autoFilter ref="A1:L18"/>
+<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:L20" insertRow="1" totalsRowShown="0">
+  <x:autoFilter ref="A1:L20"/>
   <x:tableColumns count="12">
     <x:tableColumn id="1" uniqueName="1" name="ID" dataDxfId="0"/>
     <x:tableColumn id="2" uniqueName="2" name="Start time" dataDxfId="3"/>
@@ -1477,11 +1507,87 @@
         <x:v>110</x:v>
       </x:c>
     </x:row>
+    <x:row r="19" hidden="0">
+      <x:c r="A19">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="B19" s="2">
+        <x:v>44614.5958796296</x:v>
+      </x:c>
+      <x:c r="C19" s="2">
+        <x:v>44614.5973726852</x:v>
+      </x:c>
+      <x:c r="D19" s="10" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="E19" s="10" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="F19" s="7" t="s">
+        <x:v>111</x:v>
+      </x:c>
+      <x:c r="G19" s="10" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="H19" s="10" t="s">
+        <x:v>112</x:v>
+      </x:c>
+      <x:c r="I19" s="10" t="s">
+        <x:v>113</x:v>
+      </x:c>
+      <x:c r="J19" s="10" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="K19" s="10" t="s">
+        <x:v>114</x:v>
+      </x:c>
+      <x:c r="L19" s="10" t="s">
+        <x:v>115</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="20" hidden="0">
+      <x:c r="A20">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="B20" s="2">
+        <x:v>44617.5091898148</x:v>
+      </x:c>
+      <x:c r="C20" s="2">
+        <x:v>44617.5111574074</x:v>
+      </x:c>
+      <x:c r="D20" s="10" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="E20" s="10" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="F20" s="7" t="s">
+        <x:v>116</x:v>
+      </x:c>
+      <x:c r="G20" s="10" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="H20" s="10" t="s">
+        <x:v>117</x:v>
+      </x:c>
+      <x:c r="I20" s="10" t="s">
+        <x:v>118</x:v>
+      </x:c>
+      <x:c r="J20" s="10" t="s">
+        <x:v>45</x:v>
+      </x:c>
+      <x:c r="K20" s="10" t="s">
+        <x:v>119</x:v>
+      </x:c>
+      <x:c r="L20" s="10" t="s">
+        <x:v>120</x:v>
+      </x:c>
+    </x:row>
   </x:sheetData>
   <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <x:pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <x:tableParts count="1">
-    <x:tablePart r:id="R2792c38cfca64069"/>
+    <x:tablePart r:id="R3e243399067f45b9"/>
   </x:tableParts>
 </x:worksheet>
 </file>
</xml_diff>